<commit_message>
* Added Portrait Template and associated screenshots * Updated Calendar screenshot with better looking image
</commit_message>
<xml_diff>
--- a/IkeaGlassBoardLayout.xlsx
+++ b/IkeaGlassBoardLayout.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="1"/>
+    <workbookView xWindow="5040" yWindow="0" windowWidth="28800" windowHeight="13020"/>
   </bookViews>
   <sheets>
-    <sheet name="Template" sheetId="1" r:id="rId1"/>
-    <sheet name="Calendar" sheetId="4" r:id="rId2"/>
-    <sheet name="Today" sheetId="5" r:id="rId3"/>
-    <sheet name="Scrum Board" sheetId="3" r:id="rId4"/>
+    <sheet name="Template Landscape" sheetId="1" r:id="rId1"/>
+    <sheet name="Template Portrait" sheetId="6" r:id="rId2"/>
+    <sheet name="Calendar" sheetId="4" r:id="rId3"/>
+    <sheet name="Today" sheetId="5" r:id="rId4"/>
+    <sheet name="Scrum Board" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="1">
   <si>
     <t>x</t>
   </si>
@@ -397,7 +398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EB91"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1985,9 +1986,1679 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:CM132"/>
+  <sheetViews>
+    <sheetView zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="DC195" sqref="DC195"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="90" width="2.85546875" customWidth="1"/>
+    <col min="91" max="91" width="2.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" s="5">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1">
+        <v>10</v>
+      </c>
+      <c r="L1" s="5">
+        <v>11</v>
+      </c>
+      <c r="M1" s="5">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1">
+        <v>14</v>
+      </c>
+      <c r="P1" s="5">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="5">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1">
+        <v>18</v>
+      </c>
+      <c r="T1" s="5">
+        <v>19</v>
+      </c>
+      <c r="U1" s="5">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1">
+        <v>22</v>
+      </c>
+      <c r="X1" s="5">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="5">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="5">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="5">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="5">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="5">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="5">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="5">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="5">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="5">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="5">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="5">
+        <v>44</v>
+      </c>
+      <c r="AT1" s="1">
+        <v>45</v>
+      </c>
+      <c r="AU1" s="1">
+        <v>46</v>
+      </c>
+      <c r="AV1" s="5">
+        <v>47</v>
+      </c>
+      <c r="AW1" s="5">
+        <v>48</v>
+      </c>
+      <c r="AX1" s="1">
+        <v>49</v>
+      </c>
+      <c r="AY1" s="1">
+        <v>50</v>
+      </c>
+      <c r="AZ1" s="5">
+        <v>51</v>
+      </c>
+      <c r="BA1" s="5">
+        <v>52</v>
+      </c>
+      <c r="BB1" s="1">
+        <v>53</v>
+      </c>
+      <c r="BC1" s="1">
+        <v>54</v>
+      </c>
+      <c r="BD1" s="5">
+        <v>55</v>
+      </c>
+      <c r="BE1" s="5">
+        <v>56</v>
+      </c>
+      <c r="BF1" s="1">
+        <v>57</v>
+      </c>
+      <c r="BG1" s="1">
+        <v>58</v>
+      </c>
+      <c r="BH1" s="5">
+        <v>59</v>
+      </c>
+      <c r="BI1" s="5">
+        <v>60</v>
+      </c>
+      <c r="BJ1" s="1">
+        <v>61</v>
+      </c>
+      <c r="BK1" s="1">
+        <v>62</v>
+      </c>
+      <c r="BL1" s="5">
+        <v>63</v>
+      </c>
+      <c r="BM1" s="5">
+        <v>64</v>
+      </c>
+      <c r="BN1" s="1">
+        <v>65</v>
+      </c>
+      <c r="BO1" s="1">
+        <v>66</v>
+      </c>
+      <c r="BP1" s="5">
+        <v>67</v>
+      </c>
+      <c r="BQ1" s="5">
+        <v>68</v>
+      </c>
+      <c r="BR1" s="1">
+        <v>69</v>
+      </c>
+      <c r="BS1" s="1">
+        <v>70</v>
+      </c>
+      <c r="BT1" s="5">
+        <v>71</v>
+      </c>
+      <c r="BU1" s="5">
+        <v>72</v>
+      </c>
+      <c r="BV1" s="1">
+        <v>73</v>
+      </c>
+      <c r="BW1" s="1">
+        <v>74</v>
+      </c>
+      <c r="BX1" s="5">
+        <v>75</v>
+      </c>
+      <c r="BY1" s="5">
+        <v>76</v>
+      </c>
+      <c r="BZ1" s="1">
+        <v>77</v>
+      </c>
+      <c r="CA1" s="1">
+        <v>78</v>
+      </c>
+      <c r="CB1" s="5">
+        <v>79</v>
+      </c>
+      <c r="CC1" s="5">
+        <v>80</v>
+      </c>
+      <c r="CD1" s="1">
+        <v>81</v>
+      </c>
+      <c r="CE1" s="1">
+        <v>82</v>
+      </c>
+      <c r="CF1" s="5">
+        <v>83</v>
+      </c>
+      <c r="CG1" s="5">
+        <v>84</v>
+      </c>
+      <c r="CH1" s="1">
+        <v>85</v>
+      </c>
+      <c r="CI1" s="1">
+        <v>86</v>
+      </c>
+      <c r="CJ1" s="5">
+        <v>87</v>
+      </c>
+      <c r="CK1" s="5">
+        <v>88</v>
+      </c>
+      <c r="CL1" s="1">
+        <v>89</v>
+      </c>
+      <c r="CM1" s="1"/>
+    </row>
+    <row r="2" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="CM2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="CM3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="CM4" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="CM5" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="CM6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="CM7" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="CC8" s="2"/>
+      <c r="CD8" s="2"/>
+      <c r="CE8" s="2"/>
+      <c r="CF8" s="2"/>
+      <c r="CM8" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="CC9" s="2"/>
+      <c r="CD9" s="2"/>
+      <c r="CE9" s="2"/>
+      <c r="CF9" s="2"/>
+      <c r="CM9" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="CC10" s="2"/>
+      <c r="CD10" s="2"/>
+      <c r="CE10" s="2"/>
+      <c r="CF10" s="2"/>
+      <c r="CM10" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="CC11" s="2"/>
+      <c r="CD11" s="2"/>
+      <c r="CE11" s="2"/>
+      <c r="CF11" s="2"/>
+      <c r="CM11" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="CM12" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="CM13" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="CM14" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="CM15" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="CM16" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="CM17" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="CM18" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="CM19" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="CM20" s="5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>20</v>
+      </c>
+      <c r="CM21" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="CM22" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="CM23" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
+      <c r="CM24" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>24</v>
+      </c>
+      <c r="CM25" s="5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="CM26" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="CM27" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>27</v>
+      </c>
+      <c r="CM28" s="5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>28</v>
+      </c>
+      <c r="CM29" s="5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="CM30" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="CM31" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>31</v>
+      </c>
+      <c r="CM32" s="5">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>32</v>
+      </c>
+      <c r="CM33" s="5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="CM34" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="CM35" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>35</v>
+      </c>
+      <c r="CM36" s="5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <v>36</v>
+      </c>
+      <c r="CM37" s="5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="CM38" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="CM39" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
+        <v>39</v>
+      </c>
+      <c r="CM40" s="5">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A41" s="5">
+        <v>40</v>
+      </c>
+      <c r="CM41" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>41</v>
+      </c>
+      <c r="CM42" s="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="CM43" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A44" s="5">
+        <v>43</v>
+      </c>
+      <c r="CM44" s="5">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A45" s="5">
+        <v>44</v>
+      </c>
+      <c r="CM45" s="5">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>45</v>
+      </c>
+      <c r="CM46" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>46</v>
+      </c>
+      <c r="CM47" s="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A48" s="5">
+        <v>47</v>
+      </c>
+      <c r="CM48" s="5">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A49" s="5">
+        <v>48</v>
+      </c>
+      <c r="CM49" s="5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>49</v>
+      </c>
+      <c r="CM50" s="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>50</v>
+      </c>
+      <c r="CM51" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A52" s="5">
+        <v>51</v>
+      </c>
+      <c r="CM52" s="5">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A53" s="5">
+        <v>52</v>
+      </c>
+      <c r="CM53" s="5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>53</v>
+      </c>
+      <c r="CM54" s="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>54</v>
+      </c>
+      <c r="CM55" s="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A56" s="5">
+        <v>55</v>
+      </c>
+      <c r="CM56" s="5">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A57" s="5">
+        <v>56</v>
+      </c>
+      <c r="CM57" s="5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>57</v>
+      </c>
+      <c r="CM58" s="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>58</v>
+      </c>
+      <c r="CM59" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A60" s="5">
+        <v>59</v>
+      </c>
+      <c r="CM60" s="5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A61" s="5">
+        <v>60</v>
+      </c>
+      <c r="CM61" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>61</v>
+      </c>
+      <c r="CM62" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>62</v>
+      </c>
+      <c r="CM63" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A64" s="5">
+        <v>63</v>
+      </c>
+      <c r="CM64" s="5">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A65" s="5">
+        <v>64</v>
+      </c>
+      <c r="CM65" s="5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>65</v>
+      </c>
+      <c r="CM66" s="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>66</v>
+      </c>
+      <c r="CM67" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A68" s="5">
+        <v>67</v>
+      </c>
+      <c r="CM68" s="5">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A69" s="5">
+        <v>68</v>
+      </c>
+      <c r="CM69" s="5">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>69</v>
+      </c>
+      <c r="CM70" s="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>70</v>
+      </c>
+      <c r="CM71" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A72" s="5">
+        <v>71</v>
+      </c>
+      <c r="CM72" s="5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A73" s="5">
+        <v>72</v>
+      </c>
+      <c r="CM73" s="5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>73</v>
+      </c>
+      <c r="CM74" s="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>74</v>
+      </c>
+      <c r="CM75" s="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A76" s="5">
+        <v>75</v>
+      </c>
+      <c r="CM76" s="5">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A77" s="5">
+        <v>76</v>
+      </c>
+      <c r="CM77" s="5">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>77</v>
+      </c>
+      <c r="CM78" s="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>78</v>
+      </c>
+      <c r="CM79" s="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A80" s="5">
+        <v>79</v>
+      </c>
+      <c r="CM80" s="5">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A81" s="5">
+        <v>80</v>
+      </c>
+      <c r="CM81" s="5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>81</v>
+      </c>
+      <c r="CM82" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>82</v>
+      </c>
+      <c r="CM83" s="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A84" s="5">
+        <v>83</v>
+      </c>
+      <c r="CM84" s="5">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A85" s="5">
+        <v>84</v>
+      </c>
+      <c r="CM85" s="5">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>85</v>
+      </c>
+      <c r="CM86" s="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>86</v>
+      </c>
+      <c r="CM87" s="1">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A88" s="5">
+        <v>87</v>
+      </c>
+      <c r="CM88" s="5">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A89" s="5">
+        <v>88</v>
+      </c>
+      <c r="CM89" s="5">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>89</v>
+      </c>
+      <c r="CM90" s="1">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>90</v>
+      </c>
+      <c r="CM91" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A92" s="5">
+        <v>91</v>
+      </c>
+      <c r="CM92" s="5">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A93" s="5">
+        <v>92</v>
+      </c>
+      <c r="CM93" s="5">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>93</v>
+      </c>
+      <c r="CM94" s="1">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>94</v>
+      </c>
+      <c r="CM95" s="1">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A96" s="5">
+        <v>95</v>
+      </c>
+      <c r="CM96" s="5">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A97" s="5">
+        <v>96</v>
+      </c>
+      <c r="CM97" s="5">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>97</v>
+      </c>
+      <c r="CM98" s="1">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>98</v>
+      </c>
+      <c r="CM99" s="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A100" s="5">
+        <v>99</v>
+      </c>
+      <c r="CM100" s="5">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A101" s="5">
+        <v>100</v>
+      </c>
+      <c r="CM101" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>101</v>
+      </c>
+      <c r="CM102" s="1">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <v>102</v>
+      </c>
+      <c r="CM103" s="1">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A104" s="5">
+        <v>103</v>
+      </c>
+      <c r="CM104" s="5">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A105" s="5">
+        <v>104</v>
+      </c>
+      <c r="CM105" s="5">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <v>105</v>
+      </c>
+      <c r="CM106" s="1">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <v>106</v>
+      </c>
+      <c r="CM107" s="1">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A108" s="5">
+        <v>107</v>
+      </c>
+      <c r="CM108" s="5">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A109" s="5">
+        <v>108</v>
+      </c>
+      <c r="CM109" s="5">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <v>109</v>
+      </c>
+      <c r="CM110" s="1">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <v>110</v>
+      </c>
+      <c r="CM111" s="1">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A112" s="5">
+        <v>111</v>
+      </c>
+      <c r="CM112" s="5">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A113" s="5">
+        <v>112</v>
+      </c>
+      <c r="CM113" s="5">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <v>113</v>
+      </c>
+      <c r="CM114" s="1">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="115" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <v>114</v>
+      </c>
+      <c r="CM115" s="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="116" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A116" s="5">
+        <v>115</v>
+      </c>
+      <c r="CM116" s="5">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="117" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A117" s="5">
+        <v>116</v>
+      </c>
+      <c r="CM117" s="5">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="118" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A118" s="1">
+        <v>117</v>
+      </c>
+      <c r="CM118" s="1">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="119" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
+        <v>118</v>
+      </c>
+      <c r="CM119" s="1">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="120" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A120" s="5">
+        <v>119</v>
+      </c>
+      <c r="CM120" s="5">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="121" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A121" s="5">
+        <v>120</v>
+      </c>
+      <c r="CM121" s="5">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="122" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A122" s="1">
+        <v>121</v>
+      </c>
+      <c r="H122" s="2"/>
+      <c r="I122" s="2"/>
+      <c r="J122" s="2"/>
+      <c r="K122" s="2"/>
+      <c r="CC122" s="2"/>
+      <c r="CD122" s="2"/>
+      <c r="CE122" s="2"/>
+      <c r="CF122" s="2"/>
+      <c r="CM122" s="1">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="123" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A123" s="1">
+        <v>122</v>
+      </c>
+      <c r="H123" s="2"/>
+      <c r="I123" s="2"/>
+      <c r="J123" s="2"/>
+      <c r="K123" s="2"/>
+      <c r="CC123" s="2"/>
+      <c r="CD123" s="2"/>
+      <c r="CE123" s="2"/>
+      <c r="CF123" s="2"/>
+      <c r="CM123" s="1">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="124" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A124" s="5">
+        <v>123</v>
+      </c>
+      <c r="H124" s="2"/>
+      <c r="I124" s="2"/>
+      <c r="J124" s="2"/>
+      <c r="K124" s="2"/>
+      <c r="CC124" s="2"/>
+      <c r="CD124" s="2"/>
+      <c r="CE124" s="2"/>
+      <c r="CF124" s="2"/>
+      <c r="CM124" s="5">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A125" s="5">
+        <v>124</v>
+      </c>
+      <c r="H125" s="2"/>
+      <c r="I125" s="2"/>
+      <c r="J125" s="2"/>
+      <c r="K125" s="2"/>
+      <c r="CC125" s="2"/>
+      <c r="CD125" s="2"/>
+      <c r="CE125" s="2"/>
+      <c r="CF125" s="2"/>
+      <c r="CM125" s="5">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="126" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A126" s="1">
+        <v>125</v>
+      </c>
+      <c r="CM126" s="1">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="127" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A127" s="1">
+        <v>126</v>
+      </c>
+      <c r="CM127" s="1">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="128" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A128" s="5">
+        <v>127</v>
+      </c>
+      <c r="CM128" s="5">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="129" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A129" s="5">
+        <v>128</v>
+      </c>
+      <c r="CM129" s="5">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A130" s="1">
+        <v>129</v>
+      </c>
+      <c r="CM130" s="1">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="131" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A131" s="1">
+        <v>130</v>
+      </c>
+      <c r="CM131" s="1">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="132" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B132" s="1">
+        <v>1</v>
+      </c>
+      <c r="C132" s="1">
+        <v>2</v>
+      </c>
+      <c r="D132" s="5">
+        <v>3</v>
+      </c>
+      <c r="E132" s="5">
+        <v>4</v>
+      </c>
+      <c r="F132" s="1">
+        <v>5</v>
+      </c>
+      <c r="G132" s="1">
+        <v>6</v>
+      </c>
+      <c r="H132" s="5">
+        <v>7</v>
+      </c>
+      <c r="I132" s="5">
+        <v>8</v>
+      </c>
+      <c r="J132" s="1">
+        <v>9</v>
+      </c>
+      <c r="K132" s="1">
+        <v>10</v>
+      </c>
+      <c r="L132" s="5">
+        <v>11</v>
+      </c>
+      <c r="M132" s="5">
+        <v>12</v>
+      </c>
+      <c r="N132" s="1">
+        <v>13</v>
+      </c>
+      <c r="O132" s="1">
+        <v>14</v>
+      </c>
+      <c r="P132" s="5">
+        <v>15</v>
+      </c>
+      <c r="Q132" s="5">
+        <v>16</v>
+      </c>
+      <c r="R132" s="1">
+        <v>17</v>
+      </c>
+      <c r="S132" s="1">
+        <v>18</v>
+      </c>
+      <c r="T132" s="5">
+        <v>19</v>
+      </c>
+      <c r="U132" s="5">
+        <v>20</v>
+      </c>
+      <c r="V132" s="1">
+        <v>21</v>
+      </c>
+      <c r="W132" s="1">
+        <v>22</v>
+      </c>
+      <c r="X132" s="5">
+        <v>23</v>
+      </c>
+      <c r="Y132" s="5">
+        <v>24</v>
+      </c>
+      <c r="Z132" s="1">
+        <v>25</v>
+      </c>
+      <c r="AA132" s="1">
+        <v>26</v>
+      </c>
+      <c r="AB132" s="5">
+        <v>27</v>
+      </c>
+      <c r="AC132" s="5">
+        <v>28</v>
+      </c>
+      <c r="AD132" s="1">
+        <v>29</v>
+      </c>
+      <c r="AE132" s="1">
+        <v>30</v>
+      </c>
+      <c r="AF132" s="5">
+        <v>31</v>
+      </c>
+      <c r="AG132" s="5">
+        <v>32</v>
+      </c>
+      <c r="AH132" s="1">
+        <v>33</v>
+      </c>
+      <c r="AI132" s="1">
+        <v>34</v>
+      </c>
+      <c r="AJ132" s="5">
+        <v>35</v>
+      </c>
+      <c r="AK132" s="5">
+        <v>36</v>
+      </c>
+      <c r="AL132" s="1">
+        <v>37</v>
+      </c>
+      <c r="AM132" s="1">
+        <v>38</v>
+      </c>
+      <c r="AN132" s="5">
+        <v>39</v>
+      </c>
+      <c r="AO132" s="5">
+        <v>40</v>
+      </c>
+      <c r="AP132" s="1">
+        <v>41</v>
+      </c>
+      <c r="AQ132" s="1">
+        <v>42</v>
+      </c>
+      <c r="AR132" s="5">
+        <v>43</v>
+      </c>
+      <c r="AS132" s="5">
+        <v>44</v>
+      </c>
+      <c r="AT132" s="1">
+        <v>45</v>
+      </c>
+      <c r="AU132" s="1">
+        <v>46</v>
+      </c>
+      <c r="AV132" s="5">
+        <v>47</v>
+      </c>
+      <c r="AW132" s="5">
+        <v>48</v>
+      </c>
+      <c r="AX132" s="1">
+        <v>49</v>
+      </c>
+      <c r="AY132" s="1">
+        <v>50</v>
+      </c>
+      <c r="AZ132" s="5">
+        <v>51</v>
+      </c>
+      <c r="BA132" s="5">
+        <v>52</v>
+      </c>
+      <c r="BB132" s="1">
+        <v>53</v>
+      </c>
+      <c r="BC132" s="1">
+        <v>54</v>
+      </c>
+      <c r="BD132" s="5">
+        <v>55</v>
+      </c>
+      <c r="BE132" s="5">
+        <v>56</v>
+      </c>
+      <c r="BF132" s="1">
+        <v>57</v>
+      </c>
+      <c r="BG132" s="1">
+        <v>58</v>
+      </c>
+      <c r="BH132" s="5">
+        <v>59</v>
+      </c>
+      <c r="BI132" s="5">
+        <v>60</v>
+      </c>
+      <c r="BJ132" s="1">
+        <v>61</v>
+      </c>
+      <c r="BK132" s="1">
+        <v>62</v>
+      </c>
+      <c r="BL132" s="5">
+        <v>63</v>
+      </c>
+      <c r="BM132" s="5">
+        <v>64</v>
+      </c>
+      <c r="BN132" s="1">
+        <v>65</v>
+      </c>
+      <c r="BO132" s="1">
+        <v>66</v>
+      </c>
+      <c r="BP132" s="5">
+        <v>67</v>
+      </c>
+      <c r="BQ132" s="5">
+        <v>68</v>
+      </c>
+      <c r="BR132" s="1">
+        <v>69</v>
+      </c>
+      <c r="BS132" s="1">
+        <v>70</v>
+      </c>
+      <c r="BT132" s="5">
+        <v>71</v>
+      </c>
+      <c r="BU132" s="5">
+        <v>72</v>
+      </c>
+      <c r="BV132" s="1">
+        <v>73</v>
+      </c>
+      <c r="BW132" s="1">
+        <v>74</v>
+      </c>
+      <c r="BX132" s="5">
+        <v>75</v>
+      </c>
+      <c r="BY132" s="5">
+        <v>76</v>
+      </c>
+      <c r="BZ132" s="1">
+        <v>77</v>
+      </c>
+      <c r="CA132" s="1">
+        <v>78</v>
+      </c>
+      <c r="CB132" s="5">
+        <v>79</v>
+      </c>
+      <c r="CC132" s="5">
+        <v>80</v>
+      </c>
+      <c r="CD132" s="1">
+        <v>81</v>
+      </c>
+      <c r="CE132" s="1">
+        <v>82</v>
+      </c>
+      <c r="CF132" s="5">
+        <v>83</v>
+      </c>
+      <c r="CG132" s="5">
+        <v>84</v>
+      </c>
+      <c r="CH132" s="1">
+        <v>85</v>
+      </c>
+      <c r="CI132" s="1">
+        <v>86</v>
+      </c>
+      <c r="CJ132" s="5">
+        <v>87</v>
+      </c>
+      <c r="CK132" s="5">
+        <v>88</v>
+      </c>
+      <c r="CL132" s="1">
+        <v>89</v>
+      </c>
+      <c r="CM132" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EB91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>
@@ -5061,7 +6732,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EB91"/>
   <sheetViews>
@@ -8513,7 +10184,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EB91"/>
   <sheetViews>

</xml_diff>